<commit_message>
Agregar un modificador para FileChooser personalizado para evitar errores al acceder a archivos devido a lectura de archivos protegidos del sistema. + DATA UPDATE
</commit_message>
<xml_diff>
--- a/REVs/REV-04-04-2025.xlsx
+++ b/REVs/REV-04-04-2025.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R118"/>
+  <dimension ref="A1:R150"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
       <selection activeCell="G102" sqref="G102"/>
@@ -6013,14 +6013,1524 @@
           <t>Revisado y Traducido</t>
         </is>
       </c>
-      <c r="K118" t="inlineStr"/>
-      <c r="L118" t="inlineStr"/>
-      <c r="M118" t="inlineStr"/>
-      <c r="N118" t="inlineStr"/>
-      <c r="O118" t="inlineStr"/>
-      <c r="P118" t="inlineStr"/>
-      <c r="Q118" t="inlineStr"/>
-      <c r="R118" t="inlineStr"/>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>0TF26701</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>BONNYHILL B VITAMIN-C SERUM</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="H119" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J119" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>0TF26702</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>BONNYHILL FOOT CREAM 100ML</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>VARIOS</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="H120" t="inlineStr">
+        <is>
+          <t>ML</t>
+        </is>
+      </c>
+      <c r="J120" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>0TS04122</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>ZIAJA SET RUTINA AUTOBRONCEADOR</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>TRAT.SOLAR</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="H121" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J121" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>2BG01773</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>ZIAJA CUPUAZU JABON CRISTALINO BAÑO &amp; DUCHA 500ML</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>TRAT.SOLAR</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J122" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>2BL02930</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>ZIAJA CUPUAZU LOCION CORPORAL BRONCEADORA 300ML</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>TRAT.SOLAR</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J123" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>0TN00932</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>ZIAJA CUPUAZU EXFOLIANTE DE AZUCAR CRISTALINO 200M</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>TRAT.SOLAR</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H124" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J124" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>0TS03888</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>ZIAJA SOLAR CREMA FACIAL BRONCEADORA BRONZE 50ML</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>TRAT.SOLAR</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H125" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J125" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>2CC02909</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>ORIGINAL REMEDIES CHAMPU  5 PLANTAS 300 ML</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H126" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J126" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>2CC05860</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>ORIGINAL REMEDIES CHAMPU 5 PLANTAS 400ML</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H127" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J127" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>2CC05858</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>ORIGINAL REMEDIES CHAMPU AGUA ARROZ 400ML</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H128" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J128" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>2CC02914</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>ORIGINAL REMEDIES CHAMPU AGUA COCO &amp; ALOE 300 ML</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H129" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J129" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>2CC05853</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>ORIGINAL REMEDIES CHAMPU AGUA COCO 400ML</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H130" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J130" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>2CC05606</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>ORIGINAL REMEDIES CHAMPU AGUA DE ARROZ 300ML</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J131" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>2CC02904</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>ORIGINAL REMEDIES CHAMPU AGUACATE &amp; KARITE 300 ML</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H132" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J132" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>2CC05854</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>ORIGINAL REMEDIES CHAMPU AGUACATE 400ML</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H133" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J133" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>2CC02908</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>ORIGINAL REMEDIES CHAMPU ARCILLA &amp; LIMON 300 ML</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H134" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J134" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>2CC05855</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>ORIGINAL REMEDIES CHAMPU ARGAN 400ML</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H135" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J135" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>2CC05862</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>ORIGINAL REMEDIES CHAMPU AVENA 400ML</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J136" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>2CC02911</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>ORIGINAL REMEDIES CHAMPU AVENA DELICATESSE 300 ML</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J137" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>2CC05857</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>ORIGINAL REMEDIES CHAMPU CAMOMILA 400ML</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J138" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>2CC04848</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>ORIGINAL REMEDIES CHAMPU CARBON 300ML</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H139" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J139" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>2CC05863</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>ORIGINAL REMEDIES CHAMPU CARBON 400ML</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H140" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J140" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>2CC05019</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>ORIGINAL REMEDIES CHAMPU CHARCOAL 250ML</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H141" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J141" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>2CC02903</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>ORIGINAL REMEDIES CHAMPU ELIXIR ARGAN 300 ML</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H142" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J142" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>2CC05861</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>ORIGINAL REMEDIES CHAMPU LIMON 400ML</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H143" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J143" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>2CC02910</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>ORIGINAL REMEDIES CHAMPU MIEL 300 ML</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H144" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J144" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>2CC05859</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>ORIGINAL REMEDIES CHAMPU MIEL 400ML</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H145" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J145" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>2CC05856</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>ORIGINAL REMEDIES CHAMPU OLIVA 400ML</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H146" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J146" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>2CC02912</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>ORIGINAL REMEDIES CHAMPU OLIVA MITICA 300 ML</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H147" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J147" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>2CC05918</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>HERBAL CHAMPU COCO PACK 2X350ML</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H148" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="J148" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>2CC05919</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>HERBAL DESIRE ROSE PACK CH350ML+MASC500ML</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H149" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I149" t="inlineStr">
+        <is>
+          <t>"8700216211086","8700216200547"</t>
+        </is>
+      </c>
+      <c r="J149" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>2CC05680</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>HERBAL BIO RENEW CHAMPU ROSA 350ML</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Tiene PT</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H150" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I150" t="inlineStr"/>
+      <c r="J150" t="inlineStr">
+        <is>
+          <t>Solo Revisión</t>
+        </is>
+      </c>
+      <c r="K150" t="inlineStr"/>
+      <c r="L150" t="inlineStr"/>
+      <c r="M150" t="inlineStr"/>
+      <c r="N150" t="inlineStr"/>
+      <c r="O150" t="inlineStr"/>
+      <c r="P150" t="inlineStr"/>
+      <c r="Q150" t="inlineStr"/>
+      <c r="R150" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Agregar funcionalidad de búsqueda (en db.db Sqlite) en el campo "Marca/Titulo"
</commit_message>
<xml_diff>
--- a/REVs/REV-04-04-2025.xlsx
+++ b/REVs/REV-04-04-2025.xlsx
@@ -415,7 +415,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R150"/>
+  <dimension ref="A1:R151"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
       <selection activeCell="G102" sqref="G102"/>
@@ -7517,20 +7517,67 @@
           <t>UND</t>
         </is>
       </c>
-      <c r="I150" t="inlineStr"/>
       <c r="J150" t="inlineStr">
         <is>
           <t>Solo Revisión</t>
         </is>
       </c>
-      <c r="K150" t="inlineStr"/>
-      <c r="L150" t="inlineStr"/>
-      <c r="M150" t="inlineStr"/>
-      <c r="N150" t="inlineStr"/>
-      <c r="O150" t="inlineStr"/>
-      <c r="P150" t="inlineStr"/>
-      <c r="Q150" t="inlineStr"/>
-      <c r="R150" t="inlineStr"/>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>0TF04311</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>L-OCCITANE GLOSS ROSE PETALE 15ML.</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>CABELLO CHAMPU</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>No Tiene PT - TRADUZIDO</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>Tiene ES</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>No Tiene IT - TRADOTTO</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="H151" t="inlineStr">
+        <is>
+          <t>UND</t>
+        </is>
+      </c>
+      <c r="I151" t="inlineStr"/>
+      <c r="J151" t="inlineStr">
+        <is>
+          <t>Revisado y Traducido</t>
+        </is>
+      </c>
+      <c r="K151" t="inlineStr"/>
+      <c r="L151" t="inlineStr"/>
+      <c r="M151" t="inlineStr"/>
+      <c r="N151" t="inlineStr"/>
+      <c r="O151" t="inlineStr"/>
+      <c r="P151" t="inlineStr"/>
+      <c r="Q151" t="inlineStr"/>
+      <c r="R151" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>